<commit_message>
added requested features. CSS improvements maybe?
</commit_message>
<xml_diff>
--- a/product list.xlsx
+++ b/product list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Season 7\FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CFF4478-77AD-4C5F-B76F-A6AF28CDF1C9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AE3B75BB-6703-4293-9014-71856607BFC3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11340" xr2:uid="{B3CB3B34-9BE4-4409-8250-C1A2A9A2AD08}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="33">
   <si>
     <t xml:space="preserve">Asus </t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>CHINA</t>
+  </si>
+  <si>
+    <t>K1L203</t>
+  </si>
+  <si>
+    <t>K2P032</t>
+  </si>
+  <si>
+    <t>Q20F55</t>
+  </si>
+  <si>
+    <t>UI032P</t>
+  </si>
+  <si>
+    <t>SEALED</t>
   </si>
 </sst>
 </file>
@@ -460,15 +475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{128AF097-0DF5-4697-A3E7-B6DC31AC4922}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -501,8 +516,11 @@
       <c r="G4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -512,8 +530,8 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>28</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -524,8 +542,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -535,8 +556,8 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6">
-        <v>2</v>
+      <c r="D6" t="s">
+        <v>29</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -548,7 +569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -558,8 +579,8 @@
       <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7">
-        <v>3</v>
+      <c r="D7" t="s">
+        <v>30</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -570,8 +591,11 @@
       <c r="G7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -581,8 +605,8 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="D8">
-        <v>4</v>
+      <c r="D8" t="s">
+        <v>29</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -594,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -604,8 +628,8 @@
       <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="D9">
-        <v>1</v>
+      <c r="D9" t="s">
+        <v>30</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
@@ -616,8 +640,11 @@
       <c r="G9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -627,8 +654,8 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10">
-        <v>2</v>
+      <c r="D10" t="s">
+        <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -640,7 +667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -650,8 +677,8 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D11">
-        <v>3</v>
+      <c r="D11" t="s">
+        <v>31</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -662,8 +689,11 @@
       <c r="G11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -673,8 +703,8 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12">
-        <v>4</v>
+      <c r="D12" t="s">
+        <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>22</v>
@@ -686,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -696,8 +726,8 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13">
-        <v>1</v>
+      <c r="D13" t="s">
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
@@ -708,8 +738,11 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -719,8 +752,8 @@
       <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="D14">
-        <v>2</v>
+      <c r="D14" t="s">
+        <v>31</v>
       </c>
       <c r="E14" t="s">
         <v>22</v>
@@ -732,7 +765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -742,8 +775,8 @@
       <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="D15">
-        <v>3</v>
+      <c r="D15" t="s">
+        <v>28</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -754,8 +787,11 @@
       <c r="G15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -765,8 +801,8 @@
       <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D16">
-        <v>4</v>
+      <c r="D16" t="s">
+        <v>30</v>
       </c>
       <c r="E16" t="s">
         <v>22</v>

</xml_diff>